<commit_message>
updated terminal to savona
</commit_message>
<xml_diff>
--- a/terminal_throughput.xlsx
+++ b/terminal_throughput.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHK\Documents\Projekte\China_European Ports\European-Ports-Ownership\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D7AD9E-1CC2-488E-BD59-B6E5C69D7631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table 1'!$A$1:$E$304</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -77,9 +78,6 @@
     <t>NLRTM</t>
   </si>
   <si>
-    <t>ITGOA</t>
-  </si>
-  <si>
     <t>Vado + Reefer Terminals</t>
   </si>
   <si>
@@ -118,11 +116,14 @@
   <si>
     <t>port_code</t>
   </si>
+  <si>
+    <t>ITSVN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -170,26 +171,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -208,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -248,9 +250,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,61 +495,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="7" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" customWidth="1"/>
-    <col min="12" max="12" width="4.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.77734375" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.77734375" customWidth="1"/>
-    <col min="16" max="16" width="4.6640625" customWidth="1"/>
-    <col min="17" max="17" width="5.77734375" customWidth="1"/>
-    <col min="18" max="18" width="4.6640625" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" customWidth="1"/>
-    <col min="21" max="21" width="5.77734375" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" customWidth="1"/>
-    <col min="23" max="23" width="5.77734375" customWidth="1"/>
-    <col min="24" max="24" width="4.6640625" customWidth="1"/>
-    <col min="25" max="26" width="5.77734375" customWidth="1"/>
+    <col min="2" max="2" width="31.296875" customWidth="1"/>
+    <col min="3" max="3" width="5.796875" customWidth="1"/>
+    <col min="4" max="4" width="4.69921875" customWidth="1"/>
+    <col min="5" max="5" width="9.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.69921875" customWidth="1"/>
+    <col min="7" max="7" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.69921875" customWidth="1"/>
+    <col min="11" max="11" width="5.796875" customWidth="1"/>
+    <col min="12" max="12" width="4.69921875" customWidth="1"/>
+    <col min="13" max="13" width="5.796875" customWidth="1"/>
+    <col min="14" max="14" width="4.69921875" customWidth="1"/>
+    <col min="15" max="15" width="5.796875" customWidth="1"/>
+    <col min="16" max="16" width="4.69921875" customWidth="1"/>
+    <col min="17" max="17" width="5.796875" customWidth="1"/>
+    <col min="18" max="18" width="4.69921875" customWidth="1"/>
+    <col min="19" max="19" width="5.796875" customWidth="1"/>
+    <col min="20" max="20" width="4.69921875" customWidth="1"/>
+    <col min="21" max="21" width="5.796875" customWidth="1"/>
+    <col min="22" max="22" width="4.69921875" customWidth="1"/>
+    <col min="23" max="23" width="5.796875" customWidth="1"/>
+    <col min="24" max="24" width="4.69921875" customWidth="1"/>
+    <col min="25" max="26" width="5.796875" customWidth="1"/>
     <col min="27" max="27" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -560,9 +562,9 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -575,9 +577,9 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -592,9 +594,9 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -609,9 +611,9 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -626,9 +628,9 @@
         <v>93.6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -643,9 +645,9 @@
         <v>148.4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -660,9 +662,9 @@
         <v>173.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -677,9 +679,9 @@
         <v>183.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -694,9 +696,9 @@
         <v>180.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -711,9 +713,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -728,9 +730,9 @@
         <v>210.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -745,9 +747,9 @@
         <v>215.4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -762,9 +764,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -779,9 +781,9 @@
         <v>324.10000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -796,9 +798,9 @@
         <v>299.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -813,9 +815,9 @@
         <v>218.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -830,9 +832,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -847,9 +849,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -864,9 +866,9 @@
         <v>173.3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
@@ -881,7 +883,7 @@
         <v>169.6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -896,7 +898,7 @@
       </c>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -911,7 +913,7 @@
       </c>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -926,7 +928,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -943,9 +945,9 @@
         <v>166.1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -960,9 +962,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -977,9 +979,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -994,9 +996,9 @@
         <v>207.3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -1011,7 +1013,7 @@
         <v>227.2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>191.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>185.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1062,7 +1064,7 @@
         <v>146.6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1079,9 +1081,9 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
@@ -1096,9 +1098,9 @@
         <v>297.7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>0</v>
@@ -1113,9 +1115,9 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
@@ -1130,9 +1132,9 @@
         <v>293.89999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
@@ -1147,7 +1149,7 @@
         <v>267.3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1164,7 +1166,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>279.3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>311.39999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1215,9 +1217,9 @@
         <v>392.5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
@@ -1232,9 +1234,9 @@
         <v>287.7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
@@ -1249,9 +1251,9 @@
         <v>262.2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
@@ -1266,9 +1268,9 @@
         <v>246.8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -1283,7 +1285,7 @@
         <v>304.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>504.6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>548.6</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1336,7 @@
         <v>505.2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -1351,9 +1353,9 @@
         <v>549.70000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
@@ -1368,9 +1370,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>0</v>
@@ -1385,9 +1387,9 @@
         <v>328.8</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
         <v>0</v>
@@ -1402,9 +1404,9 @@
         <v>364.3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
@@ -1419,7 +1421,7 @@
         <v>377.5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1436,7 +1438,7 @@
         <v>535.29999999999995</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1455,7 @@
         <v>625.29999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -1470,7 +1472,7 @@
         <v>644.9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -1487,9 +1489,9 @@
         <v>714.1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B58" t="s">
         <v>0</v>
@@ -1504,9 +1506,9 @@
         <v>375.9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
         <v>0</v>
@@ -1521,9 +1523,9 @@
         <v>416.6</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B60" t="s">
         <v>0</v>
@@ -1538,9 +1540,9 @@
         <v>480.5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
@@ -1555,7 +1557,7 @@
         <v>454.1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>685.1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>785.5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>754.9</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -1624,9 +1626,9 @@
       </c>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
@@ -1641,9 +1643,9 @@
         <v>520.20000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
         <v>0</v>
@@ -1658,9 +1660,9 @@
         <v>489.5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
@@ -1675,9 +1677,9 @@
         <v>482.9</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
@@ -1692,7 +1694,7 @@
         <v>522.79999999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>736.4</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>745.3</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>771.7</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -1760,9 +1762,9 @@
         <v>781.1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
         <v>0</v>
@@ -1777,9 +1779,9 @@
         <v>484.2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -1794,9 +1796,9 @@
         <v>534.9</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B76" t="s">
         <v>0</v>
@@ -1811,9 +1813,9 @@
         <v>474</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
@@ -1828,7 +1830,7 @@
         <v>429.3</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>806.9</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -1862,7 +1864,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>956.8</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>825.3</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>11</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>199.3</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1932,7 @@
         <v>167.7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>11</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>150.19999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>11</v>
       </c>
@@ -1965,9 +1967,9 @@
       </c>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>3</v>
@@ -1982,9 +1984,9 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>3</v>
@@ -1999,9 +2001,9 @@
         <v>92.3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>3</v>
@@ -2016,9 +2018,9 @@
         <v>59.5</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>3</v>
@@ -2033,7 +2035,7 @@
         <v>40.9</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>12</v>
       </c>
@@ -2048,7 +2050,7 @@
       </c>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>12</v>
       </c>
@@ -2063,7 +2065,7 @@
       </c>
       <c r="E91" s="6"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>12</v>
       </c>
@@ -2077,7 +2079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>12</v>
       </c>
@@ -2094,9 +2096,9 @@
         <v>653.79999999999995</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
         <v>0</v>
@@ -2111,9 +2113,9 @@
         <v>469.5</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B95" t="s">
         <v>0</v>
@@ -2128,9 +2130,9 @@
         <v>565.4</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
         <v>0</v>
@@ -2145,9 +2147,9 @@
         <v>580.20000000000005</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B97" t="s">
         <v>0</v>
@@ -2162,7 +2164,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -2179,7 +2181,7 @@
         <v>833.9</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>919.7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>951.4</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>986.8</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>11</v>
       </c>
@@ -2247,7 +2249,7 @@
         <v>173.1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>11</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>240.2</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>337.1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>11</v>
       </c>
@@ -2299,9 +2301,9 @@
       </c>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B106" t="s">
         <v>3</v>
@@ -2316,9 +2318,9 @@
         <v>67.7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B107" t="s">
         <v>3</v>
@@ -2333,9 +2335,9 @@
         <v>81.7</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B108" t="s">
         <v>3</v>
@@ -2350,9 +2352,9 @@
         <v>93.7</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B109" t="s">
         <v>3</v>
@@ -2367,7 +2369,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>12</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>12</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>683.9</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>12</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>703.8</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>12</v>
       </c>
@@ -2435,9 +2437,9 @@
         <v>639.6</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>13</v>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -2449,9 +2451,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>13</v>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -2466,9 +2468,9 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>13</v>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
@@ -2483,9 +2485,9 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>13</v>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
@@ -2500,9 +2502,9 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>6</v>
@@ -2514,9 +2516,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>6</v>
@@ -2528,9 +2530,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>6</v>
@@ -2542,9 +2544,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>6</v>
@@ -2559,9 +2561,9 @@
         <v>554</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B122" t="s">
         <v>0</v>
@@ -2576,9 +2578,9 @@
         <v>570.1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
         <v>0</v>
@@ -2593,9 +2595,9 @@
         <v>593.29999999999995</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B124" t="s">
         <v>0</v>
@@ -2610,9 +2612,9 @@
         <v>557.29999999999995</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B125" t="s">
         <v>0</v>
@@ -2627,7 +2629,7 @@
         <v>509.8</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>10</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>1001.4</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -2661,7 +2663,7 @@
         <v>1074.0999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>10</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>1165.9000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>10</v>
       </c>
@@ -2695,7 +2697,7 @@
         <v>1167.7</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>11</v>
       </c>
@@ -2712,7 +2714,7 @@
         <v>311.10000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>11</v>
       </c>
@@ -2729,7 +2731,7 @@
         <v>341.1</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +2748,7 @@
         <v>316.8</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>11</v>
       </c>
@@ -2764,9 +2766,9 @@
       </c>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -2781,9 +2783,9 @@
         <v>108.4</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
@@ -2798,9 +2800,9 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
@@ -2815,9 +2817,9 @@
         <v>106.8</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
@@ -2832,7 +2834,7 @@
         <v>91.1</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>12</v>
       </c>
@@ -2849,7 +2851,7 @@
         <v>671.7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>785.9</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>12</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>796.2</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>12</v>
       </c>
@@ -2900,9 +2902,9 @@
         <v>800.3</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>13</v>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B142" t="s">
         <v>5</v>
@@ -2917,9 +2919,9 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>13</v>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B143" t="s">
         <v>5</v>
@@ -2934,9 +2936,9 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>13</v>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B144" t="s">
         <v>5</v>
@@ -2951,9 +2953,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>13</v>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B145" t="s">
         <v>5</v>
@@ -2968,9 +2970,9 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B146" t="s">
         <v>6</v>
@@ -2985,9 +2987,9 @@
         <v>829.8</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B147" t="s">
         <v>6</v>
@@ -3002,9 +3004,9 @@
         <v>932.9</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B148" t="s">
         <v>6</v>
@@ -3019,9 +3021,9 @@
         <v>943.6</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B149" t="s">
         <v>6</v>
@@ -3036,9 +3038,9 @@
         <v>916</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B150" t="s">
         <v>0</v>
@@ -3053,9 +3055,9 @@
         <v>519</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B151" t="s">
         <v>0</v>
@@ -3070,9 +3072,9 @@
         <v>556.9</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B152" t="s">
         <v>0</v>
@@ -3087,9 +3089,9 @@
         <v>514.29999999999995</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B153" t="s">
         <v>0</v>
@@ -3104,7 +3106,7 @@
         <v>519.1</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -3121,7 +3123,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>1323.9</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -3155,7 +3157,7 @@
         <v>1342.4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3174,7 @@
         <v>1246.3</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>11</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>292.60000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>11</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>322.8</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>11</v>
       </c>
@@ -3223,7 +3225,7 @@
         <v>342.7</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>11</v>
       </c>
@@ -3241,9 +3243,9 @@
       </c>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B162" t="s">
         <v>7</v>
@@ -3258,9 +3260,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B163" t="s">
         <v>7</v>
@@ -3275,9 +3277,9 @@
         <v>95.7</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B164" t="s">
         <v>7</v>
@@ -3292,9 +3294,9 @@
         <v>143.4</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B165" t="s">
         <v>7</v>
@@ -3309,7 +3311,7 @@
         <v>155.5</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>12</v>
       </c>
@@ -3326,7 +3328,7 @@
         <v>754.4</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>12</v>
       </c>
@@ -3343,7 +3345,7 @@
         <v>765.6</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>12</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>12</v>
       </c>
@@ -3377,9 +3379,9 @@
         <v>629</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
-        <v>13</v>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
@@ -3394,9 +3396,9 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>13</v>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
@@ -3411,9 +3413,9 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
-        <v>13</v>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A172" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B172" t="s">
         <v>5</v>
@@ -3428,9 +3430,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>13</v>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A173" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B173" t="s">
         <v>5</v>
@@ -3445,9 +3447,9 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>8</v>
@@ -3462,9 +3464,9 @@
         <v>923.4</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
@@ -3479,9 +3481,9 @@
         <v>988.4</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
@@ -3496,9 +3498,9 @@
         <v>886.1</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
@@ -3513,9 +3515,9 @@
         <v>787.3</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B178" t="s">
         <v>0</v>
@@ -3530,9 +3532,9 @@
         <v>508.9</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B179" t="s">
         <v>0</v>
@@ -3547,9 +3549,9 @@
         <v>524.20000000000005</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B180" t="s">
         <v>0</v>
@@ -3564,9 +3566,9 @@
         <v>607.4</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B181" t="s">
         <v>0</v>
@@ -3581,7 +3583,7 @@
         <v>625.9</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>10</v>
       </c>
@@ -3598,7 +3600,7 @@
         <v>1215.9000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3617,7 @@
         <v>1193.5</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>10</v>
       </c>
@@ -3632,7 +3634,7 @@
         <v>1287.0999999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>10</v>
       </c>
@@ -3649,7 +3651,7 @@
         <v>1200.4000000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>11</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>307.8</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>11</v>
       </c>
@@ -3683,7 +3685,7 @@
         <v>294.60000000000002</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>11</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>294.8</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>11</v>
       </c>
@@ -3718,9 +3720,9 @@
       </c>
       <c r="H189" s="1"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -3735,9 +3737,9 @@
         <v>153.19999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
@@ -3752,9 +3754,9 @@
         <v>139.30000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B192" t="s">
         <v>7</v>
@@ -3769,9 +3771,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -3786,7 +3788,7 @@
         <v>175.7</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>12</v>
       </c>
@@ -3803,7 +3805,7 @@
         <v>600.6</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>12</v>
       </c>
@@ -3820,7 +3822,7 @@
         <v>546.79999999999995</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>12</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>623.5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>12</v>
       </c>
@@ -3854,9 +3856,9 @@
         <v>683.7</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>13</v>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
@@ -3871,9 +3873,9 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>13</v>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
@@ -3888,9 +3890,9 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
-        <v>13</v>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B200" t="s">
         <v>5</v>
@@ -3905,9 +3907,9 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>13</v>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="B201" t="s">
         <v>5</v>
@@ -3922,9 +3924,9 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
@@ -3939,9 +3941,9 @@
         <v>801.3</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B203" t="s">
         <v>8</v>
@@ -3956,9 +3958,9 @@
         <v>747.2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B204" t="s">
         <v>8</v>
@@ -3973,9 +3975,9 @@
         <v>910.4</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
@@ -3990,9 +3992,9 @@
         <v>928.9</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B206" t="s">
         <v>0</v>
@@ -4007,9 +4009,9 @@
         <v>541.5</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B207" t="s">
         <v>0</v>
@@ -4024,9 +4026,9 @@
         <v>575.29999999999995</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B208" t="s">
         <v>0</v>
@@ -4041,9 +4043,9 @@
         <v>527.79999999999995</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B209" t="s">
         <v>0</v>
@@ -4058,7 +4060,7 @@
         <v>557.9</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>10</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>10</v>
       </c>
@@ -4092,7 +4094,7 @@
         <v>1225.9000000000001</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>10</v>
       </c>
@@ -4109,7 +4111,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>10</v>
       </c>
@@ -4126,7 +4128,7 @@
         <v>1035.4000000000001</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>11</v>
       </c>
@@ -4143,7 +4145,7 @@
         <v>305.39999999999998</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>11</v>
       </c>
@@ -4160,7 +4162,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>11</v>
       </c>
@@ -4177,7 +4179,7 @@
         <v>307.2</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>11</v>
       </c>
@@ -4195,9 +4197,9 @@
       </c>
       <c r="H217" s="1"/>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B218" t="s">
         <v>7</v>
@@ -4212,9 +4214,9 @@
         <v>218.9</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B219" t="s">
         <v>7</v>
@@ -4229,9 +4231,9 @@
         <v>214.2</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B220" t="s">
         <v>7</v>
@@ -4246,9 +4248,9 @@
         <v>245.3</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B221" t="s">
         <v>7</v>
@@ -4263,7 +4265,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>12</v>
       </c>
@@ -4280,7 +4282,7 @@
         <v>640.70000000000005</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>12</v>
       </c>
@@ -4297,7 +4299,7 @@
         <v>692.2</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>12</v>
       </c>
@@ -4314,7 +4316,7 @@
         <v>667.8</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>12</v>
       </c>
@@ -4331,7 +4333,7 @@
         <v>657.4</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B226" t="s">
         <v>5</v>
       </c>
@@ -4345,7 +4347,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B227" t="s">
         <v>5</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B228" t="s">
         <v>5</v>
       </c>
@@ -4373,7 +4375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B229" t="s">
         <v>5</v>
       </c>
@@ -4387,7 +4389,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
         <v>9</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B231" t="s">
         <v>9</v>
       </c>
@@ -4409,7 +4411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B232" t="s">
         <v>9</v>
       </c>
@@ -4420,7 +4422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B233" t="s">
         <v>9</v>
       </c>
@@ -4434,12 +4436,12 @@
         <v>56.7</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" s="2" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A234" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B234" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B234" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C234">
         <v>2021</v>
@@ -4452,12 +4454,12 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="2" t="s">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A235" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B235" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B235" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C235">
         <v>2021</v>
@@ -4470,12 +4472,12 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="2" t="s">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A236" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B236" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B236" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C236">
         <v>2021</v>
@@ -4488,12 +4490,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" s="2" t="s">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B237" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B237" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C237">
         <v>2021</v>
@@ -4506,9 +4508,9 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B238" t="s">
         <v>8</v>
@@ -4523,9 +4525,9 @@
         <v>860.9</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
@@ -4540,9 +4542,9 @@
         <v>918.6</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B240" t="s">
         <v>8</v>
@@ -4557,9 +4559,9 @@
         <v>916.8</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
@@ -4574,9 +4576,9 @@
         <v>924.9</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B242" t="s">
         <v>0</v>
@@ -4591,9 +4593,9 @@
         <v>540.4</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B243" t="s">
         <v>0</v>
@@ -4608,9 +4610,9 @@
         <v>536.1</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B244" t="s">
         <v>0</v>
@@ -4625,9 +4627,9 @@
         <v>528.20000000000005</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B245" t="s">
         <v>0</v>
@@ -4642,7 +4644,7 @@
         <v>503.1</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>10</v>
       </c>
@@ -4659,7 +4661,7 @@
         <v>1089.0999999999999</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>10</v>
       </c>
@@ -4676,7 +4678,7 @@
         <v>1045.9000000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>10</v>
       </c>
@@ -4693,7 +4695,7 @@
         <v>1130.9000000000001</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>10</v>
       </c>
@@ -4710,7 +4712,7 @@
         <v>1077.0999999999999</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>11</v>
       </c>
@@ -4727,7 +4729,7 @@
         <v>321.5</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>11</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>291.8</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>11</v>
       </c>
@@ -4761,7 +4763,7 @@
         <v>292.8</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>11</v>
       </c>
@@ -4779,9 +4781,9 @@
       </c>
       <c r="H253" s="1"/>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B254" t="s">
         <v>7</v>
@@ -4796,9 +4798,9 @@
         <v>272.3</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B255" t="s">
         <v>7</v>
@@ -4813,9 +4815,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B256" t="s">
         <v>7</v>
@@ -4830,9 +4832,9 @@
         <v>303.2</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B257" t="s">
         <v>7</v>
@@ -4847,7 +4849,7 @@
         <v>220.2</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>12</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>662.2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>12</v>
       </c>
@@ -4881,7 +4883,7 @@
         <v>675.3</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>12</v>
       </c>
@@ -4898,7 +4900,7 @@
         <v>648.6</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>12</v>
       </c>
@@ -4915,7 +4917,7 @@
         <v>657.9</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B262" t="s">
         <v>5</v>
       </c>
@@ -4929,7 +4931,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B263" t="s">
         <v>5</v>
       </c>
@@ -4943,7 +4945,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B264" t="s">
         <v>5</v>
       </c>
@@ -4957,7 +4959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B265" t="s">
         <v>5</v>
       </c>
@@ -4971,7 +4973,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B266" t="s">
         <v>9</v>
       </c>
@@ -4985,7 +4987,7 @@
         <v>44.9</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B267" t="s">
         <v>9</v>
       </c>
@@ -4999,7 +5001,7 @@
         <v>52.8</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B268" t="s">
         <v>9</v>
       </c>
@@ -5013,7 +5015,7 @@
         <v>51.2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B269" t="s">
         <v>9</v>
       </c>
@@ -5027,12 +5029,12 @@
         <v>73.5</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270" s="2" t="s">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A270" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B270" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B270" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C270">
         <v>2022</v>
@@ -5045,12 +5047,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="2" t="s">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A271" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B271" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B271" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C271">
         <v>2022</v>
@@ -5063,12 +5065,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272" s="2" t="s">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A272" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B272" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B272" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C272">
         <v>2022</v>
@@ -5081,12 +5083,12 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" s="2" t="s">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A273" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B273" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B273" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C273">
         <v>2022</v>
@@ -5099,9 +5101,9 @@
         <v>89.2</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B274" t="s">
         <v>8</v>
@@ -5116,9 +5118,9 @@
         <v>892</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B275" t="s">
         <v>8</v>
@@ -5133,9 +5135,9 @@
         <v>936.2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B276" t="s">
         <v>8</v>
@@ -5150,9 +5152,9 @@
         <v>901.1</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B277" t="s">
         <v>8</v>
@@ -5167,9 +5169,9 @@
         <v>701.5</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B278" t="s">
         <v>0</v>
@@ -5184,9 +5186,9 @@
         <v>475.4</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B279" t="s">
         <v>0</v>
@@ -5201,9 +5203,9 @@
         <v>520.4</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B280" t="s">
         <v>0</v>
@@ -5218,7 +5220,7 @@
         <v>516.9</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>10</v>
       </c>
@@ -5235,7 +5237,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>10</v>
       </c>
@@ -5252,7 +5254,7 @@
         <v>1197.2</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>10</v>
       </c>
@@ -5269,7 +5271,7 @@
         <v>1194.5</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>11</v>
       </c>
@@ -5286,7 +5288,7 @@
         <v>327.5</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>11</v>
       </c>
@@ -5303,7 +5305,7 @@
         <v>351.6</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>11</v>
       </c>
@@ -5320,9 +5322,9 @@
         <v>346.6</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B287" t="s">
         <v>7</v>
@@ -5337,9 +5339,9 @@
         <v>149.9</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B288" t="s">
         <v>7</v>
@@ -5354,9 +5356,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B289" t="s">
         <v>7</v>
@@ -5371,7 +5373,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>12</v>
       </c>
@@ -5388,7 +5390,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>12</v>
       </c>
@@ -5405,7 +5407,7 @@
         <v>642.70000000000005</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>12</v>
       </c>
@@ -5422,7 +5424,7 @@
         <v>636.5</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="2"/>
       <c r="B293" t="s">
         <v>5</v>
@@ -5437,7 +5439,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B294" t="s">
         <v>5</v>
       </c>
@@ -5451,7 +5453,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B295" t="s">
         <v>5</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B296" t="s">
         <v>9</v>
       </c>
@@ -5479,7 +5481,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B297" t="s">
         <v>9</v>
       </c>
@@ -5493,7 +5495,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B298" t="s">
         <v>9</v>
       </c>
@@ -5507,12 +5509,12 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="2" t="s">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A299" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B299" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B299" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C299">
         <v>2023</v>
@@ -5525,12 +5527,12 @@
         <v>83.800000000000011</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="2" t="s">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A300" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B300" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B300" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C300">
         <v>2023</v>
@@ -5543,12 +5545,12 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="2" t="s">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A301" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B301" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B301" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C301">
         <v>2023</v>
@@ -5561,9 +5563,9 @@
         <v>97.899999999999991</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B302" t="s">
         <v>8</v>
@@ -5578,9 +5580,9 @@
         <v>733.5</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B303" t="s">
         <v>8</v>
@@ -5595,9 +5597,9 @@
         <v>809.8</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B304" t="s">
         <v>8</v>
@@ -5612,7 +5614,7 @@
         <v>787.5</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" s="2"/>
     </row>
   </sheetData>
@@ -5622,33 +5624,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.8984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>